<commit_message>
Add Link-PP LPJ1026AGNL Ethernet jack
</commit_message>
<xml_diff>
--- a/BeagleBoard-xM_BOM.xlsx
+++ b/BeagleBoard-xM_BOM.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="316">
   <si>
     <t>BEAGLE-xM PCB ASSEMBLY BOM</t>
   </si>
@@ -127,7 +127,7 @@
     <t>C3</t>
   </si>
   <si>
-    <t>Changed POP Memory Part number, changed PMIC part number, updated rev notes to C3 and small layout change to improve manufacturing yield</t>
+    <t>Changed POP Memory Part number, changed PMIC part number, added Ethernet connector, updated rev notes to C3 and small layout change to improve manufacturing yield</t>
   </si>
   <si>
     <t>JK</t>
@@ -530,6 +530,9 @@
   </si>
   <si>
     <t>0817-1A1T-11-F</t>
+  </si>
+  <si>
+    <t>LPJ1026AGNL</t>
   </si>
   <si>
     <t>TRANS ARRAY PNP/PNP W/RES S MINI</t>
@@ -1467,26 +1470,26 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1504,7 +1507,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1537,7 +1540,7 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1573,8 +1576,8 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
@@ -1699,9 +1702,6 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1735,9 +1735,6 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
@@ -1762,16 +1759,16 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="5" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1943,13 +1940,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -2039,7 +2030,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2048,10 +2039,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -2306,13 +2297,7 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -2616,7 +2601,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2625,10 +2610,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -2879,7 +2864,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J130"/>
+  <dimension ref="A1:J131"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -3310,14 +3295,14 @@
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
     </row>
-    <row r="27" ht="13.65" customHeight="1">
+    <row r="27" ht="24.65" customHeight="1">
       <c r="A27" t="s" s="22">
         <v>37</v>
       </c>
-      <c r="B27" t="s" s="32">
+      <c r="B27" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="C27" s="35"/>
+      <c r="C27" s="33"/>
       <c r="D27" s="34">
         <v>42628</v>
       </c>
@@ -4359,9 +4344,9 @@
         <v>2</v>
       </c>
       <c r="F77" s="23"/>
-      <c r="G77" s="77"/>
-      <c r="H77" s="77"/>
-      <c r="I77" s="77"/>
+      <c r="G77" s="6"/>
+      <c r="H77" s="6"/>
+      <c r="I77" s="6"/>
       <c r="J77" s="6"/>
     </row>
     <row r="78" ht="13.65" customHeight="1">
@@ -4387,21 +4372,13 @@
       <c r="J78" s="6"/>
     </row>
     <row r="79" ht="13.65" customHeight="1">
-      <c r="A79" s="51">
-        <v>40</v>
-      </c>
-      <c r="B79" t="s" s="78">
+      <c r="A79" s="53"/>
+      <c r="B79" s="53"/>
+      <c r="C79" s="53"/>
+      <c r="D79" t="s" s="61">
         <v>173</v>
       </c>
-      <c r="C79" t="s" s="78">
-        <v>174</v>
-      </c>
-      <c r="D79" t="s" s="54">
-        <v>175</v>
-      </c>
-      <c r="E79" s="72">
-        <v>2</v>
-      </c>
+      <c r="E79" s="53"/>
       <c r="F79" s="23"/>
       <c r="G79" s="6"/>
       <c r="H79" s="6"/>
@@ -4409,37 +4386,35 @@
       <c r="J79" s="6"/>
     </row>
     <row r="80" ht="13.65" customHeight="1">
-      <c r="A80" s="57"/>
-      <c r="B80" s="79"/>
-      <c r="C80" s="79"/>
+      <c r="A80" s="51">
+        <v>40</v>
+      </c>
+      <c r="B80" t="s" s="77">
+        <v>174</v>
+      </c>
+      <c r="C80" t="s" s="77">
+        <v>175</v>
+      </c>
       <c r="D80" t="s" s="54">
         <v>176</v>
       </c>
-      <c r="E80" s="74"/>
+      <c r="E80" s="72">
+        <v>2</v>
+      </c>
       <c r="F80" s="23"/>
       <c r="G80" s="6"/>
       <c r="H80" s="6"/>
       <c r="I80" s="6"/>
-      <c r="J80" t="s" s="55">
-        <v>40</v>
-      </c>
+      <c r="J80" s="6"/>
     </row>
     <row r="81" ht="13.65" customHeight="1">
-      <c r="A81" s="51">
-        <v>41</v>
-      </c>
-      <c r="B81" t="s" s="59">
+      <c r="A81" s="57"/>
+      <c r="B81" s="78"/>
+      <c r="C81" s="78"/>
+      <c r="D81" t="s" s="54">
         <v>177</v>
       </c>
-      <c r="C81" t="s" s="59">
-        <v>178</v>
-      </c>
-      <c r="D81" t="s" s="54">
-        <v>179</v>
-      </c>
-      <c r="E81" s="58">
-        <v>4</v>
-      </c>
+      <c r="E81" s="74"/>
       <c r="F81" s="23"/>
       <c r="G81" s="6"/>
       <c r="H81" s="6"/>
@@ -4449,42 +4424,44 @@
       </c>
     </row>
     <row r="82" ht="13.65" customHeight="1">
-      <c r="A82" s="58">
-        <v>42</v>
+      <c r="A82" s="51">
+        <v>41</v>
       </c>
       <c r="B82" t="s" s="59">
+        <v>178</v>
+      </c>
+      <c r="C82" t="s" s="59">
+        <v>179</v>
+      </c>
+      <c r="D82" t="s" s="54">
         <v>180</v>
       </c>
-      <c r="C82" t="s" s="59">
-        <v>181</v>
-      </c>
-      <c r="D82" t="s" s="54">
-        <v>182</v>
-      </c>
       <c r="E82" s="58">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F82" s="23"/>
       <c r="G82" s="6"/>
       <c r="H82" s="6"/>
       <c r="I82" s="6"/>
-      <c r="J82" s="6"/>
+      <c r="J82" t="s" s="55">
+        <v>40</v>
+      </c>
     </row>
     <row r="83" ht="13.65" customHeight="1">
-      <c r="A83" s="51">
-        <v>43</v>
+      <c r="A83" s="58">
+        <v>42</v>
       </c>
       <c r="B83" t="s" s="59">
+        <v>181</v>
+      </c>
+      <c r="C83" t="s" s="59">
+        <v>182</v>
+      </c>
+      <c r="D83" t="s" s="54">
         <v>183</v>
       </c>
-      <c r="C83" t="s" s="59">
-        <v>184</v>
-      </c>
-      <c r="D83" t="s" s="54">
-        <v>185</v>
-      </c>
       <c r="E83" s="58">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F83" s="23"/>
       <c r="G83" s="6"/>
@@ -4492,45 +4469,45 @@
       <c r="I83" s="6"/>
       <c r="J83" s="6"/>
     </row>
-    <row r="84" ht="20.7" customHeight="1">
-      <c r="A84" s="58">
-        <v>44</v>
-      </c>
-      <c r="B84" t="s" s="62">
+    <row r="84" ht="13.65" customHeight="1">
+      <c r="A84" s="51">
+        <v>43</v>
+      </c>
+      <c r="B84" t="s" s="59">
+        <v>184</v>
+      </c>
+      <c r="C84" t="s" s="59">
+        <v>185</v>
+      </c>
+      <c r="D84" t="s" s="54">
         <v>186</v>
       </c>
-      <c r="C84" t="s" s="63">
-        <v>187</v>
-      </c>
-      <c r="D84" t="s" s="54">
-        <v>188</v>
-      </c>
       <c r="E84" s="58">
-        <v>38</v>
-      </c>
-      <c r="F84" s="65"/>
+        <v>7</v>
+      </c>
+      <c r="F84" s="23"/>
       <c r="G84" s="6"/>
       <c r="H84" s="6"/>
       <c r="I84" s="6"/>
       <c r="J84" s="6"/>
     </row>
-    <row r="85" ht="13.65" customHeight="1">
-      <c r="A85" s="51">
-        <v>45</v>
-      </c>
-      <c r="B85" t="s" s="59">
+    <row r="85" ht="20.7" customHeight="1">
+      <c r="A85" s="58">
+        <v>44</v>
+      </c>
+      <c r="B85" t="s" s="62">
+        <v>187</v>
+      </c>
+      <c r="C85" t="s" s="63">
+        <v>188</v>
+      </c>
+      <c r="D85" t="s" s="54">
         <v>189</v>
       </c>
-      <c r="C85" t="s" s="59">
-        <v>190</v>
-      </c>
-      <c r="D85" t="s" s="61">
-        <v>191</v>
-      </c>
       <c r="E85" s="58">
-        <v>1</v>
-      </c>
-      <c r="F85" s="23"/>
+        <v>38</v>
+      </c>
+      <c r="F85" s="65"/>
       <c r="G85" s="6"/>
       <c r="H85" s="6"/>
       <c r="I85" s="6"/>
@@ -4538,16 +4515,16 @@
     </row>
     <row r="86" ht="13.65" customHeight="1">
       <c r="A86" s="51">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B86" t="s" s="59">
+        <v>190</v>
+      </c>
+      <c r="C86" t="s" s="59">
+        <v>191</v>
+      </c>
+      <c r="D86" t="s" s="61">
         <v>192</v>
-      </c>
-      <c r="C86" t="s" s="59">
-        <v>193</v>
-      </c>
-      <c r="D86" t="s" s="54">
-        <v>194</v>
       </c>
       <c r="E86" s="58">
         <v>1</v>
@@ -4560,19 +4537,19 @@
     </row>
     <row r="87" ht="13.65" customHeight="1">
       <c r="A87" s="51">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B87" t="s" s="59">
+        <v>193</v>
+      </c>
+      <c r="C87" t="s" s="59">
+        <v>194</v>
+      </c>
+      <c r="D87" t="s" s="54">
         <v>195</v>
       </c>
-      <c r="C87" t="s" s="59">
-        <v>196</v>
-      </c>
-      <c r="D87" t="s" s="80">
-        <v>197</v>
-      </c>
       <c r="E87" s="58">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F87" s="23"/>
       <c r="G87" s="6"/>
@@ -4580,45 +4557,45 @@
       <c r="I87" s="6"/>
       <c r="J87" s="6"/>
     </row>
-    <row r="88" ht="11.25" customHeight="1">
-      <c r="A88" s="58">
-        <v>48</v>
-      </c>
-      <c r="B88" t="s" s="56">
+    <row r="88" ht="13.65" customHeight="1">
+      <c r="A88" s="51">
+        <v>47</v>
+      </c>
+      <c r="B88" t="s" s="59">
+        <v>196</v>
+      </c>
+      <c r="C88" t="s" s="59">
+        <v>197</v>
+      </c>
+      <c r="D88" t="s" s="79">
         <v>198</v>
       </c>
-      <c r="C88" t="s" s="62">
-        <v>199</v>
-      </c>
-      <c r="D88" t="s" s="54">
-        <v>200</v>
-      </c>
       <c r="E88" s="58">
-        <v>1</v>
-      </c>
-      <c r="F88" s="65"/>
+        <v>3</v>
+      </c>
+      <c r="F88" s="23"/>
       <c r="G88" s="6"/>
       <c r="H88" s="6"/>
       <c r="I88" s="6"/>
       <c r="J88" s="6"/>
     </row>
-    <row r="89" ht="13.65" customHeight="1">
-      <c r="A89" s="51">
-        <v>49</v>
-      </c>
-      <c r="B89" t="s" s="59">
+    <row r="89" ht="11.25" customHeight="1">
+      <c r="A89" s="58">
+        <v>48</v>
+      </c>
+      <c r="B89" t="s" s="56">
+        <v>199</v>
+      </c>
+      <c r="C89" t="s" s="62">
+        <v>200</v>
+      </c>
+      <c r="D89" t="s" s="54">
         <v>201</v>
-      </c>
-      <c r="C89" t="s" s="59">
-        <v>202</v>
-      </c>
-      <c r="D89" t="s" s="54">
-        <v>203</v>
       </c>
       <c r="E89" s="58">
         <v>1</v>
       </c>
-      <c r="F89" s="23"/>
+      <c r="F89" s="65"/>
       <c r="G89" s="6"/>
       <c r="H89" s="6"/>
       <c r="I89" s="6"/>
@@ -4626,16 +4603,16 @@
     </row>
     <row r="90" ht="13.65" customHeight="1">
       <c r="A90" s="51">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B90" t="s" s="59">
+        <v>202</v>
+      </c>
+      <c r="C90" t="s" s="59">
+        <v>203</v>
+      </c>
+      <c r="D90" t="s" s="54">
         <v>204</v>
-      </c>
-      <c r="C90" t="s" s="59">
-        <v>205</v>
-      </c>
-      <c r="D90" t="s" s="61">
-        <v>206</v>
       </c>
       <c r="E90" s="58">
         <v>1</v>
@@ -4648,19 +4625,19 @@
     </row>
     <row r="91" ht="13.65" customHeight="1">
       <c r="A91" s="51">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B91" t="s" s="59">
+        <v>205</v>
+      </c>
+      <c r="C91" t="s" s="59">
+        <v>206</v>
+      </c>
+      <c r="D91" t="s" s="61">
         <v>207</v>
       </c>
-      <c r="C91" t="s" s="59">
-        <v>208</v>
-      </c>
-      <c r="D91" t="s" s="54">
-        <v>209</v>
-      </c>
       <c r="E91" s="58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F91" s="23"/>
       <c r="G91" s="6"/>
@@ -4670,19 +4647,19 @@
     </row>
     <row r="92" ht="13.65" customHeight="1">
       <c r="A92" s="51">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B92" t="s" s="59">
+        <v>208</v>
+      </c>
+      <c r="C92" t="s" s="59">
+        <v>209</v>
+      </c>
+      <c r="D92" t="s" s="54">
         <v>210</v>
       </c>
-      <c r="C92" t="s" s="59">
-        <v>211</v>
-      </c>
-      <c r="D92" t="s" s="61">
-        <v>212</v>
-      </c>
       <c r="E92" s="58">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F92" s="23"/>
       <c r="G92" s="6"/>
@@ -4692,19 +4669,19 @@
     </row>
     <row r="93" ht="13.65" customHeight="1">
       <c r="A93" s="51">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B93" t="s" s="59">
+        <v>211</v>
+      </c>
+      <c r="C93" t="s" s="59">
+        <v>212</v>
+      </c>
+      <c r="D93" t="s" s="61">
         <v>213</v>
       </c>
-      <c r="C93" t="s" s="59">
-        <v>214</v>
-      </c>
-      <c r="D93" t="s" s="54">
-        <v>215</v>
-      </c>
       <c r="E93" s="58">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F93" s="23"/>
       <c r="G93" s="6"/>
@@ -4714,19 +4691,19 @@
     </row>
     <row r="94" ht="13.65" customHeight="1">
       <c r="A94" s="51">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B94" t="s" s="59">
+        <v>214</v>
+      </c>
+      <c r="C94" t="s" s="59">
+        <v>215</v>
+      </c>
+      <c r="D94" t="s" s="54">
         <v>216</v>
       </c>
-      <c r="C94" t="s" s="59">
-        <v>217</v>
-      </c>
-      <c r="D94" t="s" s="61">
-        <v>218</v>
-      </c>
       <c r="E94" s="58">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F94" s="23"/>
       <c r="G94" s="6"/>
@@ -4736,19 +4713,19 @@
     </row>
     <row r="95" ht="13.65" customHeight="1">
       <c r="A95" s="51">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B95" t="s" s="59">
+        <v>217</v>
+      </c>
+      <c r="C95" t="s" s="59">
+        <v>218</v>
+      </c>
+      <c r="D95" t="s" s="61">
         <v>219</v>
       </c>
-      <c r="C95" t="s" s="59">
-        <v>220</v>
-      </c>
-      <c r="D95" t="s" s="61">
-        <v>221</v>
-      </c>
       <c r="E95" s="58">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F95" s="23"/>
       <c r="G95" s="6"/>
@@ -4758,19 +4735,19 @@
     </row>
     <row r="96" ht="13.65" customHeight="1">
       <c r="A96" s="51">
-        <v>56</v>
-      </c>
-      <c r="B96" t="s" s="56">
+        <v>55</v>
+      </c>
+      <c r="B96" t="s" s="59">
+        <v>220</v>
+      </c>
+      <c r="C96" t="s" s="59">
+        <v>221</v>
+      </c>
+      <c r="D96" t="s" s="61">
         <v>222</v>
       </c>
-      <c r="C96" t="s" s="59">
-        <v>223</v>
-      </c>
-      <c r="D96" t="s" s="54">
-        <v>224</v>
-      </c>
       <c r="E96" s="58">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F96" s="23"/>
       <c r="G96" s="6"/>
@@ -4780,19 +4757,19 @@
     </row>
     <row r="97" ht="13.65" customHeight="1">
       <c r="A97" s="51">
-        <v>57</v>
-      </c>
-      <c r="B97" t="s" s="59">
+        <v>56</v>
+      </c>
+      <c r="B97" t="s" s="56">
+        <v>223</v>
+      </c>
+      <c r="C97" t="s" s="59">
+        <v>224</v>
+      </c>
+      <c r="D97" t="s" s="54">
         <v>225</v>
       </c>
-      <c r="C97" t="s" s="59">
-        <v>226</v>
-      </c>
-      <c r="D97" t="s" s="54">
-        <v>227</v>
-      </c>
       <c r="E97" s="58">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F97" s="23"/>
       <c r="G97" s="6"/>
@@ -4802,19 +4779,19 @@
     </row>
     <row r="98" ht="13.65" customHeight="1">
       <c r="A98" s="51">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B98" t="s" s="59">
+        <v>226</v>
+      </c>
+      <c r="C98" t="s" s="59">
+        <v>227</v>
+      </c>
+      <c r="D98" t="s" s="54">
         <v>228</v>
       </c>
-      <c r="C98" t="s" s="59">
-        <v>229</v>
-      </c>
-      <c r="D98" t="s" s="54">
-        <v>230</v>
-      </c>
       <c r="E98" s="58">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F98" s="23"/>
       <c r="G98" s="6"/>
@@ -4824,19 +4801,19 @@
     </row>
     <row r="99" ht="13.65" customHeight="1">
       <c r="A99" s="51">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B99" t="s" s="59">
+        <v>229</v>
+      </c>
+      <c r="C99" t="s" s="59">
+        <v>230</v>
+      </c>
+      <c r="D99" t="s" s="54">
         <v>231</v>
       </c>
-      <c r="C99" t="s" s="59">
-        <v>232</v>
-      </c>
-      <c r="D99" t="s" s="54">
-        <v>233</v>
-      </c>
       <c r="E99" s="58">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F99" s="23"/>
       <c r="G99" s="6"/>
@@ -4846,19 +4823,19 @@
     </row>
     <row r="100" ht="13.65" customHeight="1">
       <c r="A100" s="51">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B100" t="s" s="59">
+        <v>232</v>
+      </c>
+      <c r="C100" t="s" s="59">
+        <v>233</v>
+      </c>
+      <c r="D100" t="s" s="54">
         <v>234</v>
       </c>
-      <c r="C100" t="s" s="59">
-        <v>235</v>
-      </c>
-      <c r="D100" t="s" s="61">
-        <v>236</v>
-      </c>
       <c r="E100" s="58">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F100" s="23"/>
       <c r="G100" s="6"/>
@@ -4868,19 +4845,19 @@
     </row>
     <row r="101" ht="13.65" customHeight="1">
       <c r="A101" s="51">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B101" t="s" s="59">
+        <v>235</v>
+      </c>
+      <c r="C101" t="s" s="59">
+        <v>236</v>
+      </c>
+      <c r="D101" t="s" s="61">
         <v>237</v>
       </c>
-      <c r="C101" t="s" s="59">
-        <v>238</v>
-      </c>
-      <c r="D101" t="s" s="61">
-        <v>239</v>
-      </c>
       <c r="E101" s="58">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F101" s="23"/>
       <c r="G101" s="6"/>
@@ -4890,19 +4867,19 @@
     </row>
     <row r="102" ht="13.65" customHeight="1">
       <c r="A102" s="51">
-        <v>62</v>
-      </c>
-      <c r="B102" t="s" s="62">
+        <v>61</v>
+      </c>
+      <c r="B102" t="s" s="59">
+        <v>238</v>
+      </c>
+      <c r="C102" t="s" s="59">
+        <v>239</v>
+      </c>
+      <c r="D102" t="s" s="61">
         <v>240</v>
       </c>
-      <c r="C102" t="s" s="59">
-        <v>241</v>
-      </c>
-      <c r="D102" t="s" s="54">
-        <v>242</v>
-      </c>
       <c r="E102" s="58">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F102" s="23"/>
       <c r="G102" s="6"/>
@@ -4912,19 +4889,19 @@
     </row>
     <row r="103" ht="13.65" customHeight="1">
       <c r="A103" s="51">
-        <v>63</v>
-      </c>
-      <c r="B103" t="s" s="59">
+        <v>62</v>
+      </c>
+      <c r="B103" t="s" s="62">
+        <v>241</v>
+      </c>
+      <c r="C103" t="s" s="59">
+        <v>242</v>
+      </c>
+      <c r="D103" t="s" s="54">
         <v>243</v>
       </c>
-      <c r="C103" t="s" s="59">
-        <v>244</v>
-      </c>
-      <c r="D103" t="s" s="54">
-        <v>245</v>
-      </c>
       <c r="E103" s="58">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F103" s="23"/>
       <c r="G103" s="6"/>
@@ -4934,19 +4911,19 @@
     </row>
     <row r="104" ht="13.65" customHeight="1">
       <c r="A104" s="51">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B104" t="s" s="59">
+        <v>244</v>
+      </c>
+      <c r="C104" t="s" s="59">
+        <v>245</v>
+      </c>
+      <c r="D104" t="s" s="54">
         <v>246</v>
       </c>
-      <c r="C104" t="s" s="59">
-        <v>247</v>
-      </c>
-      <c r="D104" t="s" s="54">
-        <v>248</v>
-      </c>
       <c r="E104" s="58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F104" s="23"/>
       <c r="G104" s="6"/>
@@ -4956,19 +4933,19 @@
     </row>
     <row r="105" ht="13.65" customHeight="1">
       <c r="A105" s="51">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B105" t="s" s="59">
+        <v>247</v>
+      </c>
+      <c r="C105" t="s" s="59">
+        <v>248</v>
+      </c>
+      <c r="D105" t="s" s="54">
         <v>249</v>
       </c>
-      <c r="C105" t="s" s="59">
-        <v>250</v>
-      </c>
-      <c r="D105" t="s" s="61">
-        <v>251</v>
-      </c>
       <c r="E105" s="58">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F105" s="23"/>
       <c r="G105" s="6"/>
@@ -4978,19 +4955,19 @@
     </row>
     <row r="106" ht="13.65" customHeight="1">
       <c r="A106" s="51">
-        <v>66</v>
-      </c>
-      <c r="B106" t="s" s="62">
+        <v>65</v>
+      </c>
+      <c r="B106" t="s" s="59">
+        <v>250</v>
+      </c>
+      <c r="C106" t="s" s="59">
+        <v>251</v>
+      </c>
+      <c r="D106" t="s" s="61">
         <v>252</v>
       </c>
-      <c r="C106" t="s" s="59">
-        <v>253</v>
-      </c>
-      <c r="D106" t="s" s="61">
-        <v>254</v>
-      </c>
       <c r="E106" s="58">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F106" s="23"/>
       <c r="G106" s="6"/>
@@ -5000,19 +4977,19 @@
     </row>
     <row r="107" ht="13.65" customHeight="1">
       <c r="A107" s="51">
-        <v>67</v>
-      </c>
-      <c r="B107" t="s" s="59">
+        <v>66</v>
+      </c>
+      <c r="B107" t="s" s="62">
+        <v>253</v>
+      </c>
+      <c r="C107" t="s" s="59">
+        <v>254</v>
+      </c>
+      <c r="D107" t="s" s="61">
         <v>255</v>
       </c>
-      <c r="C107" t="s" s="59">
-        <v>256</v>
-      </c>
-      <c r="D107" t="s" s="80">
-        <v>257</v>
-      </c>
       <c r="E107" s="58">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F107" s="23"/>
       <c r="G107" s="6"/>
@@ -5022,19 +4999,19 @@
     </row>
     <row r="108" ht="13.65" customHeight="1">
       <c r="A108" s="51">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B108" t="s" s="59">
+        <v>256</v>
+      </c>
+      <c r="C108" t="s" s="59">
+        <v>257</v>
+      </c>
+      <c r="D108" t="s" s="79">
         <v>258</v>
       </c>
-      <c r="C108" t="s" s="59">
-        <v>259</v>
-      </c>
-      <c r="D108" t="s" s="54">
-        <v>260</v>
-      </c>
       <c r="E108" s="58">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F108" s="23"/>
       <c r="G108" s="6"/>
@@ -5044,19 +5021,19 @@
     </row>
     <row r="109" ht="13.65" customHeight="1">
       <c r="A109" s="51">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B109" t="s" s="59">
+        <v>259</v>
+      </c>
+      <c r="C109" t="s" s="59">
+        <v>260</v>
+      </c>
+      <c r="D109" t="s" s="54">
         <v>261</v>
       </c>
-      <c r="C109" t="s" s="59">
-        <v>262</v>
-      </c>
-      <c r="D109" t="s" s="61">
-        <v>263</v>
-      </c>
       <c r="E109" s="58">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F109" s="23"/>
       <c r="G109" s="6"/>
@@ -5064,21 +5041,21 @@
       <c r="I109" s="6"/>
       <c r="J109" s="6"/>
     </row>
-    <row r="110" ht="12" customHeight="1">
+    <row r="110" ht="13.65" customHeight="1">
       <c r="A110" s="51">
-        <v>70</v>
-      </c>
-      <c r="B110" t="s" s="76">
+        <v>69</v>
+      </c>
+      <c r="B110" t="s" s="59">
+        <v>262</v>
+      </c>
+      <c r="C110" t="s" s="59">
+        <v>263</v>
+      </c>
+      <c r="D110" t="s" s="61">
         <v>264</v>
       </c>
-      <c r="C110" t="s" s="59">
-        <v>265</v>
-      </c>
-      <c r="D110" t="s" s="61">
-        <v>266</v>
-      </c>
       <c r="E110" s="58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F110" s="23"/>
       <c r="G110" s="6"/>
@@ -5086,21 +5063,21 @@
       <c r="I110" s="6"/>
       <c r="J110" s="6"/>
     </row>
-    <row r="111" ht="13.65" customHeight="1">
+    <row r="111" ht="12" customHeight="1">
       <c r="A111" s="51">
-        <v>71</v>
-      </c>
-      <c r="B111" t="s" s="56">
+        <v>70</v>
+      </c>
+      <c r="B111" t="s" s="76">
+        <v>265</v>
+      </c>
+      <c r="C111" t="s" s="59">
+        <v>266</v>
+      </c>
+      <c r="D111" t="s" s="61">
         <v>267</v>
       </c>
-      <c r="C111" t="s" s="59">
-        <v>268</v>
-      </c>
-      <c r="D111" t="s" s="54">
-        <v>269</v>
-      </c>
       <c r="E111" s="58">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F111" s="23"/>
       <c r="G111" s="6"/>
@@ -5108,18 +5085,18 @@
       <c r="I111" s="6"/>
       <c r="J111" s="6"/>
     </row>
-    <row r="112" ht="11.25" customHeight="1">
+    <row r="112" ht="13.65" customHeight="1">
       <c r="A112" s="51">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B112" t="s" s="56">
+        <v>268</v>
+      </c>
+      <c r="C112" t="s" s="59">
+        <v>269</v>
+      </c>
+      <c r="D112" t="s" s="54">
         <v>270</v>
-      </c>
-      <c r="C112" t="s" s="59">
-        <v>271</v>
-      </c>
-      <c r="D112" t="s" s="80">
-        <v>272</v>
       </c>
       <c r="E112" s="58">
         <v>1</v>
@@ -5130,18 +5107,18 @@
       <c r="I112" s="6"/>
       <c r="J112" s="6"/>
     </row>
-    <row r="113" ht="13.65" customHeight="1">
+    <row r="113" ht="11.25" customHeight="1">
       <c r="A113" s="51">
-        <v>73</v>
-      </c>
-      <c r="B113" t="s" s="59">
+        <v>72</v>
+      </c>
+      <c r="B113" t="s" s="56">
+        <v>271</v>
+      </c>
+      <c r="C113" t="s" s="59">
+        <v>272</v>
+      </c>
+      <c r="D113" t="s" s="79">
         <v>273</v>
-      </c>
-      <c r="C113" t="s" s="59">
-        <v>274</v>
-      </c>
-      <c r="D113" t="s" s="61">
-        <v>275</v>
       </c>
       <c r="E113" s="58">
         <v>1</v>
@@ -5152,18 +5129,18 @@
       <c r="I113" s="6"/>
       <c r="J113" s="6"/>
     </row>
-    <row r="114" ht="13.5" customHeight="1">
+    <row r="114" ht="13.65" customHeight="1">
       <c r="A114" s="51">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B114" t="s" s="59">
+        <v>274</v>
+      </c>
+      <c r="C114" t="s" s="59">
+        <v>275</v>
+      </c>
+      <c r="D114" t="s" s="61">
         <v>276</v>
-      </c>
-      <c r="C114" t="s" s="59">
-        <v>277</v>
-      </c>
-      <c r="D114" t="s" s="80">
-        <v>278</v>
       </c>
       <c r="E114" s="58">
         <v>1</v>
@@ -5174,21 +5151,21 @@
       <c r="I114" s="6"/>
       <c r="J114" s="6"/>
     </row>
-    <row r="115" ht="13.65" customHeight="1">
+    <row r="115" ht="13.5" customHeight="1">
       <c r="A115" s="51">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B115" t="s" s="59">
+        <v>277</v>
+      </c>
+      <c r="C115" t="s" s="59">
+        <v>278</v>
+      </c>
+      <c r="D115" t="s" s="79">
         <v>279</v>
       </c>
-      <c r="C115" t="s" s="59">
-        <v>280</v>
-      </c>
-      <c r="D115" t="s" s="80">
-        <v>281</v>
-      </c>
       <c r="E115" s="58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F115" s="23"/>
       <c r="G115" s="6"/>
@@ -5198,19 +5175,19 @@
     </row>
     <row r="116" ht="13.65" customHeight="1">
       <c r="A116" s="51">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B116" t="s" s="59">
+        <v>280</v>
+      </c>
+      <c r="C116" t="s" s="59">
+        <v>281</v>
+      </c>
+      <c r="D116" t="s" s="79">
         <v>282</v>
       </c>
-      <c r="C116" t="s" s="59">
-        <v>283</v>
-      </c>
-      <c r="D116" t="s" s="61">
-        <v>284</v>
-      </c>
       <c r="E116" s="58">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F116" s="23"/>
       <c r="G116" s="6"/>
@@ -5219,17 +5196,17 @@
       <c r="J116" s="6"/>
     </row>
     <row r="117" ht="13.65" customHeight="1">
-      <c r="A117" s="58">
-        <v>77</v>
+      <c r="A117" s="51">
+        <v>76</v>
       </c>
       <c r="B117" t="s" s="59">
+        <v>283</v>
+      </c>
+      <c r="C117" t="s" s="59">
+        <v>284</v>
+      </c>
+      <c r="D117" t="s" s="61">
         <v>285</v>
-      </c>
-      <c r="C117" t="s" s="59">
-        <v>286</v>
-      </c>
-      <c r="D117" t="s" s="61">
-        <v>287</v>
       </c>
       <c r="E117" s="58">
         <v>1</v>
@@ -5241,20 +5218,20 @@
       <c r="J117" s="6"/>
     </row>
     <row r="118" ht="13.65" customHeight="1">
-      <c r="A118" s="51">
-        <v>78</v>
+      <c r="A118" s="58">
+        <v>77</v>
       </c>
       <c r="B118" t="s" s="59">
+        <v>286</v>
+      </c>
+      <c r="C118" t="s" s="59">
+        <v>287</v>
+      </c>
+      <c r="D118" t="s" s="61">
         <v>288</v>
       </c>
-      <c r="C118" t="s" s="59">
-        <v>289</v>
-      </c>
-      <c r="D118" t="s" s="61">
-        <v>290</v>
-      </c>
       <c r="E118" s="58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F118" s="23"/>
       <c r="G118" s="6"/>
@@ -5264,19 +5241,19 @@
     </row>
     <row r="119" ht="13.65" customHeight="1">
       <c r="A119" s="51">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B119" t="s" s="59">
+        <v>289</v>
+      </c>
+      <c r="C119" t="s" s="59">
+        <v>290</v>
+      </c>
+      <c r="D119" t="s" s="61">
         <v>291</v>
       </c>
-      <c r="C119" t="s" s="59">
-        <v>292</v>
-      </c>
-      <c r="D119" t="s" s="61">
-        <v>293</v>
-      </c>
       <c r="E119" s="58">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F119" s="23"/>
       <c r="G119" s="6"/>
@@ -5286,16 +5263,16 @@
     </row>
     <row r="120" ht="13.65" customHeight="1">
       <c r="A120" s="51">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B120" t="s" s="59">
+        <v>292</v>
+      </c>
+      <c r="C120" t="s" s="59">
+        <v>293</v>
+      </c>
+      <c r="D120" t="s" s="61">
         <v>294</v>
-      </c>
-      <c r="C120" t="s" s="59">
-        <v>295</v>
-      </c>
-      <c r="D120" t="s" s="61">
-        <v>296</v>
       </c>
       <c r="E120" s="58">
         <v>1</v>
@@ -5308,16 +5285,16 @@
     </row>
     <row r="121" ht="13.65" customHeight="1">
       <c r="A121" s="51">
-        <v>81</v>
-      </c>
-      <c r="B121" t="s" s="56">
+        <v>80</v>
+      </c>
+      <c r="B121" t="s" s="59">
+        <v>295</v>
+      </c>
+      <c r="C121" t="s" s="59">
+        <v>296</v>
+      </c>
+      <c r="D121" t="s" s="61">
         <v>297</v>
-      </c>
-      <c r="C121" t="s" s="59">
-        <v>298</v>
-      </c>
-      <c r="D121" t="s" s="61">
-        <v>299</v>
       </c>
       <c r="E121" s="58">
         <v>1</v>
@@ -5330,16 +5307,16 @@
     </row>
     <row r="122" ht="13.65" customHeight="1">
       <c r="A122" s="51">
-        <v>82</v>
-      </c>
-      <c r="B122" t="s" s="59">
+        <v>81</v>
+      </c>
+      <c r="B122" t="s" s="56">
+        <v>298</v>
+      </c>
+      <c r="C122" t="s" s="59">
+        <v>299</v>
+      </c>
+      <c r="D122" t="s" s="61">
         <v>300</v>
-      </c>
-      <c r="C122" t="s" s="59">
-        <v>301</v>
-      </c>
-      <c r="D122" t="s" s="61">
-        <v>302</v>
       </c>
       <c r="E122" s="58">
         <v>1</v>
@@ -5352,16 +5329,16 @@
     </row>
     <row r="123" ht="13.65" customHeight="1">
       <c r="A123" s="51">
-        <v>83</v>
-      </c>
-      <c r="B123" t="s" s="56">
+        <v>82</v>
+      </c>
+      <c r="B123" t="s" s="59">
+        <v>301</v>
+      </c>
+      <c r="C123" t="s" s="59">
+        <v>302</v>
+      </c>
+      <c r="D123" t="s" s="61">
         <v>303</v>
-      </c>
-      <c r="C123" t="s" s="59">
-        <v>304</v>
-      </c>
-      <c r="D123" t="s" s="81">
-        <v>305</v>
       </c>
       <c r="E123" s="58">
         <v>1</v>
@@ -5374,164 +5351,190 @@
     </row>
     <row r="124" ht="13.65" customHeight="1">
       <c r="A124" s="51">
-        <v>84</v>
-      </c>
-      <c r="B124" t="s" s="59">
+        <v>83</v>
+      </c>
+      <c r="B124" t="s" s="56">
+        <v>304</v>
+      </c>
+      <c r="C124" t="s" s="59">
+        <v>305</v>
+      </c>
+      <c r="D124" t="s" s="80">
         <v>306</v>
-      </c>
-      <c r="C124" t="s" s="59">
-        <v>307</v>
-      </c>
-      <c r="D124" t="s" s="61">
-        <v>308</v>
       </c>
       <c r="E124" s="58">
         <v>1</v>
       </c>
       <c r="F124" s="23"/>
-      <c r="G124" s="77"/>
-      <c r="H124" s="77"/>
-      <c r="I124" s="77"/>
+      <c r="G124" s="6"/>
+      <c r="H124" s="6"/>
+      <c r="I124" s="6"/>
       <c r="J124" s="6"/>
     </row>
     <row r="125" ht="13.65" customHeight="1">
       <c r="A125" s="51">
-        <v>85</v>
-      </c>
-      <c r="B125" t="s" s="82">
+        <v>84</v>
+      </c>
+      <c r="B125" t="s" s="59">
+        <v>307</v>
+      </c>
+      <c r="C125" t="s" s="59">
+        <v>308</v>
+      </c>
+      <c r="D125" t="s" s="61">
         <v>309</v>
-      </c>
-      <c r="C125" t="s" s="62">
-        <v>310</v>
-      </c>
-      <c r="D125" t="s" s="83">
-        <v>311</v>
       </c>
       <c r="E125" s="58">
         <v>1</v>
       </c>
-      <c r="F125" s="65"/>
+      <c r="F125" s="23"/>
       <c r="G125" s="6"/>
       <c r="H125" s="6"/>
       <c r="I125" s="6"/>
       <c r="J125" s="6"/>
     </row>
-    <row r="126" ht="8" customHeight="1">
-      <c r="A126" s="84"/>
-      <c r="B126" s="85"/>
-      <c r="C126" t="s" s="86">
-        <v>40</v>
-      </c>
-      <c r="D126" s="87"/>
-      <c r="E126" s="88"/>
-      <c r="F126" s="89"/>
+    <row r="126" ht="13.65" customHeight="1">
+      <c r="A126" s="51">
+        <v>85</v>
+      </c>
+      <c r="B126" t="s" s="81">
+        <v>310</v>
+      </c>
+      <c r="C126" t="s" s="62">
+        <v>311</v>
+      </c>
+      <c r="D126" t="s" s="82">
+        <v>312</v>
+      </c>
+      <c r="E126" s="58">
+        <v>1</v>
+      </c>
+      <c r="F126" s="65"/>
       <c r="G126" s="6"/>
       <c r="H126" s="6"/>
       <c r="I126" s="6"/>
       <c r="J126" s="6"/>
     </row>
-    <row r="127" ht="40.7" customHeight="1">
-      <c r="A127" t="s" s="90">
+    <row r="127" ht="8" customHeight="1">
+      <c r="A127" s="83"/>
+      <c r="B127" s="84"/>
+      <c r="C127" t="s" s="85">
         <v>40</v>
       </c>
-      <c r="B127" s="91"/>
-      <c r="C127" t="s" s="92">
-        <v>312</v>
-      </c>
-      <c r="D127" s="93"/>
-      <c r="E127" t="s" s="94">
-        <v>40</v>
-      </c>
-      <c r="F127" s="77"/>
+      <c r="D127" s="86"/>
+      <c r="E127" s="87"/>
+      <c r="F127" s="12"/>
       <c r="G127" s="6"/>
       <c r="H127" s="6"/>
       <c r="I127" s="6"/>
       <c r="J127" s="6"/>
     </row>
-    <row r="128" ht="8" customHeight="1">
-      <c r="A128" s="95"/>
-      <c r="B128" s="85"/>
-      <c r="C128" t="s" s="86">
+    <row r="128" ht="40.7" customHeight="1">
+      <c r="A128" t="s" s="88">
         <v>40</v>
       </c>
-      <c r="D128" s="96"/>
-      <c r="E128" s="97"/>
-      <c r="F128" s="89"/>
+      <c r="B128" s="89"/>
+      <c r="C128" t="s" s="90">
+        <v>313</v>
+      </c>
+      <c r="D128" s="91"/>
+      <c r="E128" t="s" s="92">
+        <v>40</v>
+      </c>
+      <c r="F128" s="6"/>
       <c r="G128" s="6"/>
       <c r="H128" s="6"/>
       <c r="I128" s="6"/>
       <c r="J128" s="6"/>
     </row>
-    <row r="129" ht="13.65" customHeight="1">
-      <c r="A129" s="98"/>
-      <c r="B129" s="99"/>
-      <c r="C129" t="s" s="100">
-        <v>313</v>
-      </c>
-      <c r="D129" s="101"/>
-      <c r="E129" s="98"/>
-      <c r="F129" s="77"/>
+    <row r="129" ht="8" customHeight="1">
+      <c r="A129" s="93"/>
+      <c r="B129" s="84"/>
+      <c r="C129" t="s" s="85">
+        <v>40</v>
+      </c>
+      <c r="D129" s="94"/>
+      <c r="E129" s="95"/>
+      <c r="F129" s="12"/>
       <c r="G129" s="6"/>
       <c r="H129" s="6"/>
       <c r="I129" s="6"/>
       <c r="J129" s="6"/>
     </row>
     <row r="130" ht="13.65" customHeight="1">
-      <c r="A130" s="6"/>
-      <c r="B130" s="6"/>
-      <c r="C130" t="s" s="102">
+      <c r="A130" s="96"/>
+      <c r="B130" s="97"/>
+      <c r="C130" t="s" s="98">
         <v>314</v>
       </c>
-      <c r="D130" s="6"/>
-      <c r="E130" s="6"/>
-      <c r="F130" s="77"/>
+      <c r="D130" s="99"/>
+      <c r="E130" s="96"/>
+      <c r="F130" s="6"/>
       <c r="G130" s="6"/>
       <c r="H130" s="6"/>
       <c r="I130" s="6"/>
       <c r="J130" s="6"/>
     </row>
+    <row r="131" ht="13.65" customHeight="1">
+      <c r="A131" s="6"/>
+      <c r="B131" s="6"/>
+      <c r="C131" t="s" s="100">
+        <v>315</v>
+      </c>
+      <c r="D131" s="6"/>
+      <c r="E131" s="6"/>
+      <c r="F131" s="6"/>
+      <c r="G131" s="6"/>
+      <c r="H131" s="6"/>
+      <c r="I131" s="6"/>
+      <c r="J131" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="40">
-    <mergeCell ref="D8:D17"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="A8:A17"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="A6:A7"/>
+  <mergeCells count="44">
+    <mergeCell ref="E78:E79"/>
+    <mergeCell ref="C78:C79"/>
+    <mergeCell ref="A78:A79"/>
+    <mergeCell ref="D19:D24"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B78:B79"/>
+    <mergeCell ref="E19:E24"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="E8:E17"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="A72:A73"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="E80:E81"/>
+    <mergeCell ref="E72:E73"/>
+    <mergeCell ref="C80:C81"/>
+    <mergeCell ref="B80:B81"/>
     <mergeCell ref="B72:B73"/>
     <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B79:B80"/>
-    <mergeCell ref="C79:C80"/>
-    <mergeCell ref="E79:E80"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="A72:A73"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="A19:A24"/>
-    <mergeCell ref="E72:E73"/>
-    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="A8:A17"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="C72:C73"/>
     <mergeCell ref="B29:C29"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="E8:E17"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="E19:E24"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D19:D24"/>
+    <mergeCell ref="A80:A81"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D8:D17"/>
   </mergeCells>
   <conditionalFormatting sqref="I36">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan" stopIfTrue="1">

</xml_diff>